<commit_message>
Stable; will try to make some minor changes but this is a good version
</commit_message>
<xml_diff>
--- a/data_jul4/SO-PackExport Data_1013075.xlsx
+++ b/data_jul4/SO-PackExport Data_1013075.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\data_jul4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C2AEAEA-CD72-4B26-82BC-CF82D8BB3AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4EFF56-8DDA-4C05-8FCB-E2232548AAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -645,7 +645,7 @@
   <dimension ref="A1:AP26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1433,7 +1433,9 @@
       <c r="E7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
       <c r="G7" s="2" t="s">
         <v>73</v>
       </c>
@@ -1552,7 +1554,9 @@
       <c r="E8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
       <c r="G8" s="2" t="s">
         <v>75</v>
       </c>
@@ -1671,7 +1675,9 @@
       <c r="E9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
       <c r="G9" s="2" t="s">
         <v>54</v>
       </c>
@@ -1790,7 +1796,9 @@
       <c r="E10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
       <c r="G10" s="2" t="s">
         <v>77</v>
       </c>

</xml_diff>